<commit_message>
Update parameters and file references in Comparison_DSL2.C
Changed Tau_values and Eg_values arrays to use single values, updated input data ROOT file to '7787all.root', and changed the data histogram name to 'full'. These updates likely reflect a new analysis configuration or dataset.
</commit_message>
<xml_diff>
--- a/Calc_Gamma_Recoil_Correction.xlsx
+++ b/Calc_Gamma_Recoil_Correction.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\S\CIAE_DNP_NRG\note\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Si24\root_scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A331A5-FC66-43CB-9E54-4F5CD4663532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDCFCCD-6621-44BF-9A65-49813F7F6519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9BE0492A-2FA3-4C66-B5FA-754BC23C79FC}"/>
+    <workbookView xWindow="7896" yWindow="36" windowWidth="15144" windowHeight="12000" xr2:uid="{9BE0492A-2FA3-4C66-B5FA-754BC23C79FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,7 +587,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4EA1534-9D16-41B1-8A18-30A3265468A3}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.3"/>
   <cols>
@@ -646,27 +648,27 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
-        <v>1184.2</v>
+        <v>1572.24</v>
       </c>
       <c r="B5" s="6">
         <f>E5*1000</f>
-        <v>2.1506610207603655E-2</v>
+        <v>3.7910501774636826E-2</v>
       </c>
       <c r="C5" s="4">
         <f>A5+B5</f>
-        <v>1184.2215066102076</v>
+        <v>1572.2779105017746</v>
       </c>
       <c r="D5" s="1">
         <f>A5/1000</f>
-        <v>1.1842000000000001</v>
+        <v>1.5722400000000001</v>
       </c>
       <c r="E5" s="7">
         <f>D5^2/2/$A$3/$D$2</f>
-        <v>2.1506610207603654E-5</v>
+        <v>3.791050177463683E-5</v>
       </c>
       <c r="F5" s="9">
         <f>C5/1000</f>
-        <v>1.1842215066102075</v>
+        <v>1.5722779105017746</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -692,26 +694,26 @@
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <f>C8-B8</f>
-        <v>2600.6962625033971</v>
+        <v>2347.4154851446924</v>
       </c>
       <c r="B8" s="6">
         <f>E8*1000</f>
-        <v>0.10373749660322008</v>
+        <v>8.4514855307390932E-2</v>
       </c>
       <c r="C8" s="8">
-        <v>2600.8000000000002</v>
+        <v>2347.5</v>
       </c>
       <c r="D8" s="9">
         <f>A8/1000</f>
-        <v>2.6006962625033969</v>
+        <v>2.3474154851446922</v>
       </c>
       <c r="E8" s="7">
         <f>F8^2/2/$A$3/$D$2</f>
-        <v>1.0373749660322008E-4</v>
+        <v>8.4514855307390936E-5</v>
       </c>
       <c r="F8" s="9">
         <f>C8/1000</f>
-        <v>2.6008</v>
+        <v>2.3475000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">

</xml_diff>